<commit_message>
add totals, finish code
</commit_message>
<xml_diff>
--- a/CHILD HEADCOUNT TEMP.xlsx
+++ b/CHILD HEADCOUNT TEMP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilyjiang/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilyjiang/Documents/GitHub/headcount/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD94D20-BF6D-9F43-A993-E74E61863DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976DD3EA-512B-0D47-8F73-9ED257BE530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24500" windowHeight="15680" xr2:uid="{26980621-B5FA-4C93-AE42-F99D98389EF9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24500" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,27 +18,30 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$P$39</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+  <si>
+    <t>Child Head Count</t>
+  </si>
+  <si>
+    <t>*Insert day here</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Site Name</t>
+  </si>
+  <si>
+    <t>Site Number</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
   <si>
     <t>TIME</t>
   </si>
@@ -67,25 +70,13 @@
     <t>FINAL DEPARTURE TIME</t>
   </si>
   <si>
-    <t>Child Head Count</t>
-  </si>
-  <si>
-    <t>Site Name</t>
-  </si>
-  <si>
-    <t>Site Number</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>*Insert day here</t>
-  </si>
-  <si>
-    <t>Total:</t>
-  </si>
-  <si>
     <t>STAFF NAME</t>
+  </si>
+  <si>
+    <t># OF STAFF</t>
+  </si>
+  <si>
+    <t>Eliot Upper</t>
   </si>
 </sst>
 </file>
@@ -125,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -187,6 +178,21 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -224,17 +230,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -258,22 +269,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>4956</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{024CDDAB-0307-B41F-3B40-948A3DE698F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CCD214-90B8-6BD5-5777-070287EACB0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -282,21 +293,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="139701" y="50800"/>
-          <a:ext cx="1987550" cy="946344"/>
+          <a:off x="152400" y="0"/>
+          <a:ext cx="2120900" cy="1003300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -604,23 +609,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3CD111-7A05-457C-8B12-F3934BFEF2D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="205" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" customWidth="1"/>
@@ -634,25 +639,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="M2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="M2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
     </row>
     <row r="3" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-    </row>
-    <row r="4" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" spans="2:15" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -661,69 +666,75 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="2:15" ht="6.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="2:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1638</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="2:15" ht="5.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="2:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="9">
         <v>0.25</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8">
         <v>1</v>
@@ -742,8 +753,8 @@
       <c r="B10" s="9">
         <v>0.27083333333333331</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="6"/>
       <c r="F10" s="8">
         <v>2</v>
@@ -760,10 +771,10 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="9">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="6"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="6"/>
       <c r="F11" s="8">
         <v>3</v>
@@ -782,8 +793,8 @@
       <c r="B12" s="9">
         <v>0.3125</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="6"/>
       <c r="F12" s="8">
         <v>4</v>
@@ -800,10 +811,10 @@
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="9">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8">
         <v>5</v>
@@ -820,10 +831,10 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="9">
-        <v>0.35416666666666702</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="6"/>
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="6"/>
       <c r="F14" s="8">
         <v>6</v>
@@ -842,8 +853,8 @@
       <c r="B15" s="9">
         <v>0.375</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="6"/>
       <c r="F15" s="8">
         <v>7</v>
@@ -860,10 +871,10 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="9">
-        <v>0.39583333333333298</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="6"/>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="6"/>
       <c r="F16" s="8">
         <v>8</v>
@@ -880,10 +891,10 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="9">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="6"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="6"/>
       <c r="F17" s="8">
         <v>9</v>
@@ -902,8 +913,8 @@
       <c r="B18" s="9">
         <v>0.4375</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8">
         <v>10</v>
@@ -920,10 +931,10 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="9">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="6"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="6"/>
       <c r="F19" s="8">
         <v>11</v>
@@ -940,10 +951,10 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="9">
-        <v>0.47916666666666602</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="6"/>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8">
         <v>12</v>
@@ -962,8 +973,8 @@
       <c r="B21" s="9">
         <v>0.5</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="6"/>
       <c r="F21" s="8">
         <v>13</v>
@@ -980,10 +991,10 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="9">
-        <v>0.52083333333333304</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="6"/>
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8">
         <v>14</v>
@@ -1000,10 +1011,10 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="9">
-        <v>0.54166666666666596</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="6"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="6"/>
       <c r="F23" s="8">
         <v>15</v>
@@ -1022,8 +1033,8 @@
       <c r="B24" s="9">
         <v>0.5625</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="6"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8">
         <v>16</v>
@@ -1040,10 +1051,10 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="9">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="6"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8">
         <v>17</v>
@@ -1060,10 +1071,10 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="9">
-        <v>0.60416666666666596</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="6"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="6"/>
       <c r="F26" s="8">
         <v>18</v>
@@ -1082,8 +1093,8 @@
       <c r="B27" s="9">
         <v>0.625</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="6"/>
       <c r="F27" s="8">
         <v>19</v>
@@ -1100,10 +1111,10 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="9">
-        <v>0.64583333333333304</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="6"/>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="6"/>
       <c r="F28" s="8">
         <v>20</v>
@@ -1120,10 +1131,10 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="9">
-        <v>0.66666666666666596</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="6"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="6"/>
       <c r="F29" s="8">
         <v>21</v>
@@ -1142,8 +1153,8 @@
       <c r="B30" s="9">
         <v>0.6875</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="6"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="6"/>
       <c r="F30" s="8">
         <v>22</v>
@@ -1160,10 +1171,10 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="9">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="6"/>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8">
         <v>23</v>
@@ -1180,10 +1191,10 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="9">
-        <v>0.72916666666666596</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="6"/>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="3"/>
       <c r="E32" s="6"/>
       <c r="F32" s="8">
         <v>24</v>
@@ -1202,8 +1213,8 @@
       <c r="B33" s="9">
         <v>0.75</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="6"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="6"/>
       <c r="F33" s="8">
         <v>25</v>
@@ -1220,10 +1231,10 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="9">
-        <v>0.77083333333333304</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="6"/>
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="3"/>
       <c r="E34" s="6"/>
       <c r="F34" s="8">
         <v>26</v>
@@ -1240,25 +1251,23 @@
     </row>
     <row r="35" spans="2:15" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
       <c r="E36" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="12"/>
+      <c r="H36" s="16"/>
       <c r="I36" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
@@ -1292,14 +1301,13 @@
       <c r="J39" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="M2:O3"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="G36:H36"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="87" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup scale="87" fitToHeight="0" orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>